<commit_message>
EPBDS-8406 Show warning message in case if there are columns, that can not be matched to conditions
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8411.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8411.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4ADAD3-5A7B-48DE-A025-230C10FB5739}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="12330"/>
+    <workbookView xWindow="2400" yWindow="900" windowWidth="31830" windowHeight="16965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Conditions</t>
   </si>
@@ -126,12 +132,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,9 +160,9 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,9 +178,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -202,7 +208,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -211,14 +217,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,9 +265,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,9 +300,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,9 +352,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -501,17 +544,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="37.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.42578125" collapsed="true"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -650,9 +693,9 @@
         <v>23</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -666,9 +709,6 @@
       </c>
       <c r="E34" t="s">
         <v>5</v>
-      </c>
-      <c r="F34" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -693,7 +733,7 @@
       <c r="E37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F37" t="s" s="2">
+      <c r="F37" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -704,7 +744,6 @@
       <c r="C38" t="s">
         <v>32</v>
       </c>
-      <c r="E38"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -713,7 +752,6 @@
       <c r="C39" t="s">
         <v>31</v>
       </c>
-      <c r="E39"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -728,7 +766,7 @@
       <c r="E40" t="s">
         <v>34</v>
       </c>
-      <c r="F40" t="s" s="0">
+      <c r="F40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -736,15 +774,15 @@
   <mergeCells count="4">
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B33:F33"/>
     <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -756,7 +794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>